<commit_message>
Add model and grid pickles for KNN and Q/LDA
Add model fit outputs for KNN, Q/LDA.
Add more reference docs.
Remove data sets not used for this project.
Update README
</commit_message>
<xml_diff>
--- a/ref_docs/Feature_Map_v1.xlsx
+++ b/ref_docs/Feature_Map_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarr\Documents\GitHub\ads505_business_proj\ref_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F83090-7733-475C-A69A-CA48C4268558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3801EC8-79C1-4AB9-B3E6-DE3CC8D2C145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E5FB942-D815-48B7-87F6-15AD5525091B}"/>
+    <workbookView xWindow="15" yWindow="1080" windowWidth="25005" windowHeight="13905" activeTab="1" xr2:uid="{9E5FB942-D815-48B7-87F6-15AD5525091B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="216">
   <si>
     <t>X1 net profit / total assets</t>
   </si>
@@ -686,6 +686,27 @@
   </si>
   <si>
     <t>train Y, #8a/#10a + SMOTE rebalancing</t>
+  </si>
+  <si>
+    <t>train_x02_tx_df01_eda1</t>
+  </si>
+  <si>
+    <t>train_y01_vc01_eda1</t>
+  </si>
+  <si>
+    <t>test_x02_tx_df01_eda1</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>train X, #3a + drop duplicates + drop highly correlated</t>
+  </si>
+  <si>
+    <t>train X, #3b + drop highly correlated</t>
   </si>
 </sst>
 </file>
@@ -5283,7 +5304,7 @@
   <dimension ref="D1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5322,7 +5343,7 @@
       </c>
       <c r="P2" s="1" cm="1">
         <f t="array" ref="P2">MAX(P3:P55+3)</f>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>67</v>
@@ -5366,7 +5387,7 @@
       </c>
       <c r="T3" s="1">
         <f t="shared" si="1"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="V3" s="1" t="str">
         <f>"|"&amp;D3&amp;REPT(V$2,R3)&amp;"|"</f>
@@ -5378,11 +5399,11 @@
       </c>
       <c r="X3" s="1" t="str">
         <f>F3&amp;REPT(X$2,T3)&amp;"|"</f>
-        <v>Comments                                                |</v>
+        <v>Comments                                                  |</v>
       </c>
       <c r="Y3" s="1" t="str">
         <f>V3&amp;W3&amp;X3</f>
-        <v>|Feature Set (X / Y)   |Data Frame Name                   |Comments                                                |</v>
+        <v>|Feature Set (X / Y)   |Data Frame Name                   |Comments                                                  |</v>
       </c>
     </row>
     <row r="4" spans="4:25" x14ac:dyDescent="0.25">
@@ -5408,7 +5429,7 @@
       </c>
       <c r="T4" s="1">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V4" s="1" t="str">
         <f>"|"&amp;REPT(V$1,N$2)&amp;"|"</f>
@@ -5420,11 +5441,11 @@
       </c>
       <c r="X4" s="1" t="str">
         <f>REPT(X$1,P2)&amp;"|"</f>
-        <v>--------------------------------------------------------|</v>
+        <v>----------------------------------------------------------|</v>
       </c>
       <c r="Y4" s="1" t="str">
         <f t="shared" ref="Y4:Y53" si="2">V4&amp;W4&amp;X4</f>
-        <v>|----------------------|----------------------------------|--------------------------------------------------------|</v>
+        <v>|----------------------|----------------------------------|----------------------------------------------------------|</v>
       </c>
     </row>
     <row r="5" spans="4:25" x14ac:dyDescent="0.25">
@@ -5463,7 +5484,7 @@
       </c>
       <c r="T5" s="1">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="V5" s="1" t="str">
         <f>"|"&amp;D5&amp;REPT(V$2,R5)&amp;"|"</f>
@@ -5475,11 +5496,11 @@
       </c>
       <c r="X5" s="1" t="str">
         <f>F5&amp;REPT(X$2,T5)&amp;"|"</f>
-        <v>full X data set, no transformations                     |</v>
+        <v>full X data set, no transformations                       |</v>
       </c>
       <c r="Y5" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|1                     |x01_df01                          |full X data set, no transformations                     |</v>
+        <v>|1                     |x01_df01                          |full X data set, no transformations                       |</v>
       </c>
     </row>
     <row r="6" spans="4:25" x14ac:dyDescent="0.25">
@@ -5518,7 +5539,7 @@
       </c>
       <c r="T6" s="1">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="V6" s="1" t="str">
         <f t="shared" ref="V6:V55" si="5">"|"&amp;D6&amp;REPT(V$2,R6)&amp;"|"</f>
@@ -5530,11 +5551,11 @@
       </c>
       <c r="X6" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, no transformations                             |</v>
+        <v>train X, no transformations                               |</v>
       </c>
       <c r="Y6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|2a                    |train_x01_df01                    |train X, no transformations                             |</v>
+        <v>|2a                    |train_x01_df01                    |train X, no transformations                               |</v>
       </c>
     </row>
     <row r="7" spans="4:25" x14ac:dyDescent="0.25">
@@ -5573,7 +5594,7 @@
       </c>
       <c r="T7" s="1">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="V7" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5585,11 +5606,11 @@
       </c>
       <c r="X7" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, no transformations                              |</v>
+        <v>test X, no transformations                                |</v>
       </c>
       <c r="Y7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|2b                    |test_x01_df01                     |test X, no transformations                              |</v>
+        <v>|2b                    |test_x01_df01                     |test X, no transformations                                |</v>
       </c>
     </row>
     <row r="8" spans="4:25" x14ac:dyDescent="0.25">
@@ -5628,7 +5649,7 @@
       </c>
       <c r="T8" s="1">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V8" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5640,11 +5661,11 @@
       </c>
       <c r="X8" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, near zero variance features (if any) removed   |</v>
+        <v>train X, near zero variance features (if any) removed     |</v>
       </c>
       <c r="Y8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|3a                    |train_x02_tx_df01                 |train X, near zero variance features (if any) removed   |</v>
+        <v>|3a                    |train_x02_tx_df01                 |train X, near zero variance features (if any) removed     |</v>
       </c>
     </row>
     <row r="9" spans="4:25" x14ac:dyDescent="0.25">
@@ -5683,7 +5704,7 @@
       </c>
       <c r="T9" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V9" s="1" t="str">
         <f t="shared" si="5"/>
@@ -5695,26 +5716,26 @@
       </c>
       <c r="X9" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, near zero variance features (if any) removed    |</v>
+        <v>test X, near zero variance features (if any) removed      |</v>
       </c>
       <c r="Y9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|3b                    |test_x02_tx_df01                  |test X, near zero variance features (if any) removed    |</v>
+        <v>|3b                    |test_x02_tx_df01                  |test X, near zero variance features (if any) removed      |</v>
       </c>
     </row>
     <row r="10" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D10" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>163</v>
+      <c r="D10" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>214</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #3a + remove features w/ null count &gt; N*.15', </v>
+        <v xml:space="preserve">'train X, #3a + drop duplicates + drop highly correlated', </v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="0"/>
@@ -5722,11 +5743,11 @@
       </c>
       <c r="O10" s="1">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="4"/>
@@ -5734,42 +5755,42 @@
       </c>
       <c r="S10" s="1">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="T10" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V10" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|4a                    |</v>
+        <v>|3c                    |</v>
       </c>
       <c r="W10" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df01                 |</v>
+        <v>train_x02_tx_df01_eda1            |</v>
       </c>
       <c r="X10" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #3a + remove features w/ null count &gt; N*.15    |</v>
+        <v>train X, #3a + drop duplicates + drop highly correlated   |</v>
       </c>
       <c r="Y10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|4a                    |train_x03_tx_df01                 |train X, #3a + remove features w/ null count &gt; N*.15    |</v>
+        <v>|3c                    |train_x02_tx_df01_eda1            |train X, #3a + drop duplicates + drop highly correlated   |</v>
       </c>
     </row>
     <row r="11" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D11" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>164</v>
+      <c r="D11" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test X, #3b + remove features w/ null count &gt; N*.15', </v>
+        <v xml:space="preserve">'train X, #3b + drop highly correlated', </v>
       </c>
       <c r="N11" s="1">
         <f t="shared" si="0"/>
@@ -5777,11 +5798,11 @@
       </c>
       <c r="O11" s="1">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="R11" s="1">
         <f t="shared" si="4"/>
@@ -5789,42 +5810,42 @@
       </c>
       <c r="S11" s="1">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="T11" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="V11" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|4b                    |</v>
+        <v>|3d                    |</v>
       </c>
       <c r="W11" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_x03_tx_df01                  |</v>
+        <v>test_x02_tx_df01_eda1             |</v>
       </c>
       <c r="X11" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, #3b + remove features w/ null count &gt; N*.15     |</v>
+        <v>train X, #3b + drop highly correlated                     |</v>
       </c>
       <c r="Y11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|4b                    |test_x03_tx_df01                  |test X, #3b + remove features w/ null count &gt; N*.15     |</v>
+        <v>|3d                    |test_x02_tx_df01_eda1             |train X, #3b + drop highly correlated                     |</v>
       </c>
     </row>
     <row r="12" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D12" s="6" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #4a + missing values imputed', </v>
+        <v xml:space="preserve">'train X, #3a + remove features w/ null count &gt; N*.15', </v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="0"/>
@@ -5836,7 +5857,7 @@
       </c>
       <c r="P12" s="1">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="R12" s="1">
         <f t="shared" si="4"/>
@@ -5848,38 +5869,38 @@
       </c>
       <c r="T12" s="1">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="V12" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|5a                    |</v>
+        <v>|4a                    |</v>
       </c>
       <c r="W12" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df02                 |</v>
+        <v>train_x03_tx_df01                 |</v>
       </c>
       <c r="X12" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #4a + missing values imputed                   |</v>
+        <v>train X, #3a + remove features w/ null count &gt; N*.15      |</v>
       </c>
       <c r="Y12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|5a                    |train_x03_tx_df02                 |train X, #4a + missing values imputed                   |</v>
+        <v>|4a                    |train_x03_tx_df01                 |train X, #3a + remove features w/ null count &gt; N*.15      |</v>
       </c>
     </row>
     <row r="13" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D13" s="6" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test X, #4b + missing values imputed', </v>
+        <v xml:space="preserve">'test X, #3b + remove features w/ null count &gt; N*.15', </v>
       </c>
       <c r="N13" s="1">
         <f t="shared" si="0"/>
@@ -5891,7 +5912,7 @@
       </c>
       <c r="P13" s="1">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" si="4"/>
@@ -5903,38 +5924,38 @@
       </c>
       <c r="T13" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="V13" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|5b                    |</v>
+        <v>|4b                    |</v>
       </c>
       <c r="W13" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_x03_tx_df02                  |</v>
+        <v>test_x03_tx_df01                  |</v>
       </c>
       <c r="X13" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, #4b + missing values imputed                    |</v>
+        <v>test X, #3b + remove features w/ null count &gt; N*.15       |</v>
       </c>
       <c r="Y13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|5b                    |test_x03_tx_df02                  |test X, #4b + missing values imputed                    |</v>
+        <v>|4b                    |test_x03_tx_df01                  |test X, #3b + remove features w/ null count &gt; N*.15       |</v>
       </c>
     </row>
     <row r="14" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D14" s="6" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #5a + *z*-score scaling', </v>
+        <v xml:space="preserve">'train X, #4a + missing values imputed', </v>
       </c>
       <c r="N14" s="1">
         <f t="shared" ref="N14:P55" si="7">LEN(D14)</f>
@@ -5946,7 +5967,7 @@
       </c>
       <c r="P14" s="1">
         <f t="shared" si="7"/>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="R14" s="1">
         <f t="shared" si="4"/>
@@ -5958,38 +5979,38 @@
       </c>
       <c r="T14" s="1">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="V14" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|6a                    |</v>
+        <v>|5a                    |</v>
       </c>
       <c r="W14" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df03                 |</v>
+        <v>train_x03_tx_df02                 |</v>
       </c>
       <c r="X14" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #5a + *z*-score scaling                        |</v>
+        <v>train X, #4a + missing values imputed                     |</v>
       </c>
       <c r="Y14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|6a                    |train_x03_tx_df03                 |train X, #5a + *z*-score scaling                        |</v>
+        <v>|5a                    |train_x03_tx_df02                 |train X, #4a + missing values imputed                     |</v>
       </c>
     </row>
     <row r="15" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D15" s="6" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test X, #5b + *z*-score scaling', </v>
+        <v xml:space="preserve">'test X, #4b + missing values imputed', </v>
       </c>
       <c r="N15" s="1">
         <f t="shared" si="7"/>
@@ -6001,7 +6022,7 @@
       </c>
       <c r="P15" s="1">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="R15" s="1">
         <f t="shared" si="4"/>
@@ -6013,38 +6034,38 @@
       </c>
       <c r="T15" s="1">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="V15" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|6b                    |</v>
+        <v>|5b                    |</v>
       </c>
       <c r="W15" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_x03_tx_df03                  |</v>
+        <v>test_x03_tx_df02                  |</v>
       </c>
       <c r="X15" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, #5b + *z*-score scaling                         |</v>
+        <v>test X, #4b + missing values imputed                      |</v>
       </c>
       <c r="Y15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|6b                    |test_x03_tx_df03                  |test X, #5b + *z*-score scaling                         |</v>
+        <v>|5b                    |test_x03_tx_df02                  |test X, #4b + missing values imputed                      |</v>
       </c>
     </row>
     <row r="16" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D16" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #5a + min-max scaling', </v>
+        <v xml:space="preserve">'train X, #5a + *z*-score scaling', </v>
       </c>
       <c r="N16" s="1">
         <f t="shared" si="7"/>
@@ -6056,7 +6077,7 @@
       </c>
       <c r="P16" s="1">
         <f t="shared" si="7"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R16" s="1">
         <f t="shared" si="4"/>
@@ -6072,34 +6093,34 @@
       </c>
       <c r="V16" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|7a                    |</v>
+        <v>|6a                    |</v>
       </c>
       <c r="W16" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df04                 |</v>
+        <v>train_x03_tx_df03                 |</v>
       </c>
       <c r="X16" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #5a + min-max scaling                          |</v>
+        <v>train X, #5a + *z*-score scaling                          |</v>
       </c>
       <c r="Y16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|7a                    |train_x03_tx_df04                 |train X, #5a + min-max scaling                          |</v>
+        <v>|6a                    |train_x03_tx_df03                 |train X, #5a + *z*-score scaling                          |</v>
       </c>
     </row>
     <row r="17" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D17" s="6" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test X, #5b + min-max scaling', </v>
+        <v xml:space="preserve">'test X, #5b + *z*-score scaling', </v>
       </c>
       <c r="N17" s="1">
         <f t="shared" si="7"/>
@@ -6111,7 +6132,7 @@
       </c>
       <c r="P17" s="1">
         <f t="shared" si="7"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="R17" s="1">
         <f t="shared" si="4"/>
@@ -6127,34 +6148,34 @@
       </c>
       <c r="V17" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|7b                    |</v>
+        <v>|6b                    |</v>
       </c>
       <c r="W17" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_x03_tx_df04                  |</v>
+        <v>test_x03_tx_df03                  |</v>
       </c>
       <c r="X17" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, #5b + min-max scaling                           |</v>
+        <v>test X, #5b + *z*-score scaling                           |</v>
       </c>
       <c r="Y17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|7b                    |test_x03_tx_df04                  |test X, #5b + min-max scaling                           |</v>
+        <v>|6b                    |test_x03_tx_df03                  |test X, #5b + *z*-score scaling                           |</v>
       </c>
     </row>
     <row r="18" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D18" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>185</v>
+      <c r="D18" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #5a + skew transformation', </v>
+        <v xml:space="preserve">'train X, #5a + min-max scaling', </v>
       </c>
       <c r="N18" s="1">
         <f t="shared" si="7"/>
@@ -6162,54 +6183,54 @@
       </c>
       <c r="O18" s="1">
         <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="P18" s="1">
-        <f t="shared" si="7"/>
-        <v>34</v>
-      </c>
       <c r="R18" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="S18" s="1">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="T18" s="1">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="V18" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|8a                    |</v>
+        <v>|7a                    |</v>
       </c>
       <c r="W18" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df05 (IN PROCESS)    |</v>
+        <v>train_x03_tx_df04                 |</v>
       </c>
       <c r="X18" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #5a + skew transformation                      |</v>
+        <v>train X, #5a + min-max scaling                            |</v>
       </c>
       <c r="Y18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|8a                    |train_x03_tx_df05 (IN PROCESS)    |train X, #5a + skew transformation                      |</v>
+        <v>|7a                    |train_x03_tx_df04                 |train X, #5a + min-max scaling                            |</v>
       </c>
     </row>
     <row r="19" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D19" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>186</v>
+      <c r="D19" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>180</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test X, #5b + skew transformation', </v>
+        <v xml:space="preserve">'test X, #5b + min-max scaling', </v>
       </c>
       <c r="N19" s="1">
         <f t="shared" si="7"/>
@@ -6217,54 +6238,54 @@
       </c>
       <c r="O19" s="1">
         <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="P19" s="1">
+        <f t="shared" si="7"/>
         <v>29</v>
       </c>
-      <c r="P19" s="1">
-        <f t="shared" si="7"/>
-        <v>33</v>
-      </c>
       <c r="R19" s="1">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
       <c r="S19" s="1">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="T19" s="1">
         <f t="shared" si="4"/>
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="V19" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|8b                    |</v>
+        <v>|7b                    |</v>
       </c>
       <c r="W19" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_x03_tx_df05 (IN PROCESS)     |</v>
+        <v>test_x03_tx_df04                  |</v>
       </c>
       <c r="X19" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test X, #5b + skew transformation                       |</v>
+        <v>test X, #5b + min-max scaling                             |</v>
       </c>
       <c r="Y19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|8b                    |test_x03_tx_df05 (IN PROCESS)     |test X, #5b + skew transformation                       |</v>
+        <v>|7b                    |test_x03_tx_df04                  |test X, #5b + min-max scaling                             |</v>
       </c>
     </row>
     <row r="20" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D20" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>194</v>
+      <c r="D20" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>185</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #6a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'train X, #5a + skew transformation', </v>
       </c>
       <c r="N20" s="1">
         <f t="shared" si="7"/>
@@ -6272,11 +6293,11 @@
       </c>
       <c r="O20" s="1">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="P20" s="1">
         <f t="shared" si="7"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R20" s="1">
         <f t="shared" si="4"/>
@@ -6284,7 +6305,7 @@
       </c>
       <c r="S20" s="1">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="T20" s="1">
         <f t="shared" si="4"/>
@@ -6292,34 +6313,34 @@
       </c>
       <c r="V20" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|6c                    |</v>
+        <v>|8a                    |</v>
       </c>
       <c r="W20" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df03a                |</v>
+        <v>train_x03_tx_df05 (IN PROCESS)    |</v>
       </c>
       <c r="X20" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #6a + SMOTE rebalancing                        |</v>
+        <v>train X, #5a + skew transformation                        |</v>
       </c>
       <c r="Y20" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|6c                    |train_x03_tx_df03a                |train X, #6a + SMOTE rebalancing                        |</v>
+        <v>|8a                    |train_x03_tx_df05 (IN PROCESS)    |train X, #5a + skew transformation                        |</v>
       </c>
     </row>
     <row r="21" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D21" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>195</v>
+      <c r="D21" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>186</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #7a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'test X, #5b + skew transformation', </v>
       </c>
       <c r="N21" s="1">
         <f t="shared" si="7"/>
@@ -6327,11 +6348,11 @@
       </c>
       <c r="O21" s="1">
         <f t="shared" si="7"/>
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="P21" s="1">
         <f t="shared" si="7"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R21" s="1">
         <f t="shared" si="4"/>
@@ -6339,42 +6360,42 @@
       </c>
       <c r="S21" s="1">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="T21" s="1">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V21" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|7c                    |</v>
+        <v>|8b                    |</v>
       </c>
       <c r="W21" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df04a                |</v>
+        <v>test_x03_tx_df05 (IN PROCESS)     |</v>
       </c>
       <c r="X21" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #7a + SMOTE rebalancing                        |</v>
+        <v>test X, #5b + skew transformation                         |</v>
       </c>
       <c r="Y21" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|7c                    |train_x03_tx_df04a                |train X, #7a + SMOTE rebalancing                        |</v>
+        <v>|8b                    |test_x03_tx_df05 (IN PROCESS)     |test X, #5b + skew transformation                         |</v>
       </c>
     </row>
     <row r="22" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D22" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>196</v>
+      <c r="D22" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train X, #8a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'train X, #6a + SMOTE rebalancing', </v>
       </c>
       <c r="N22" s="1">
         <f t="shared" si="7"/>
@@ -6382,7 +6403,7 @@
       </c>
       <c r="O22" s="1">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="P22" s="1">
         <f t="shared" si="7"/>
@@ -6394,207 +6415,207 @@
       </c>
       <c r="S22" s="1">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="T22" s="1">
         <f t="shared" si="4"/>
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="V22" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|8c                    |</v>
+        <v>|6c                    |</v>
       </c>
       <c r="W22" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_x03_tx_df05a (IN PROCESS)   |</v>
+        <v>train_x03_tx_df03a                |</v>
       </c>
       <c r="X22" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train X, #8a + SMOTE rebalancing                        |</v>
+        <v>train X, #6a + SMOTE rebalancing                          |</v>
       </c>
       <c r="Y22" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|8c                    |train_x03_tx_df05a (IN PROCESS)   |train X, #8a + SMOTE rebalancing                        |</v>
+        <v>|6c                    |train_x03_tx_df03a                |train X, #6a + SMOTE rebalancing                          |</v>
       </c>
     </row>
     <row r="23" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D23" s="6">
-        <v>9</v>
+      <c r="D23" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="G23" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'full Y data set, no transformations', </v>
+        <v xml:space="preserve">'train X, #7a + SMOTE rebalancing', </v>
       </c>
       <c r="N23" s="1">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="1">
         <f t="shared" si="7"/>
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="P23" s="1">
         <f t="shared" si="7"/>
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="R23" s="1">
         <f t="shared" si="4"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S23" s="1">
         <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="T23" s="1">
+        <f t="shared" si="4"/>
         <v>26</v>
-      </c>
-      <c r="T23" s="1">
-        <f t="shared" si="4"/>
-        <v>21</v>
       </c>
       <c r="V23" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|9                     |</v>
+        <v>|7c                    |</v>
       </c>
       <c r="W23" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>y01_df01                          |</v>
+        <v>train_x03_tx_df04a                |</v>
       </c>
       <c r="X23" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>full Y data set, no transformations                     |</v>
+        <v>train X, #7a + SMOTE rebalancing                          |</v>
       </c>
       <c r="Y23" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|9                     |y01_df01                          |full Y data set, no transformations                     |</v>
+        <v>|7c                    |train_x03_tx_df04a                |train X, #7a + SMOTE rebalancing                          |</v>
       </c>
     </row>
     <row r="24" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D24" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>157</v>
+      <c r="D24" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train Y, no transformations', </v>
+        <v xml:space="preserve">'train X, #8a + SMOTE rebalancing', </v>
       </c>
       <c r="N24" s="1">
         <f t="shared" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="O24" s="1">
+        <f t="shared" si="7"/>
+        <v>31</v>
+      </c>
+      <c r="P24" s="1">
+        <f t="shared" si="7"/>
+        <v>32</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="S24" s="1">
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="O24" s="1">
-        <f t="shared" si="7"/>
-        <v>14</v>
-      </c>
-      <c r="P24" s="1">
-        <f t="shared" si="7"/>
-        <v>27</v>
-      </c>
-      <c r="R24" s="1">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="S24" s="1">
-        <f t="shared" si="4"/>
-        <v>20</v>
-      </c>
       <c r="T24" s="1">
         <f t="shared" si="4"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="V24" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|10a                   |</v>
+        <v>|8c                    |</v>
       </c>
       <c r="W24" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_y01_vc01                    |</v>
+        <v>train_x03_tx_df05a (IN PROCESS)   |</v>
       </c>
       <c r="X24" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train Y, no transformations                             |</v>
+        <v>train X, #8a + SMOTE rebalancing                          |</v>
       </c>
       <c r="Y24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|10a                   |train_y01_vc01                    |train Y, no transformations                             |</v>
+        <v>|8c                    |train_x03_tx_df05a (IN PROCESS)   |train X, #8a + SMOTE rebalancing                          |</v>
       </c>
     </row>
     <row r="25" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D25" s="6" t="s">
-        <v>188</v>
+      <c r="D25" s="6">
+        <v>9</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'test Y, no transformations', </v>
+        <v xml:space="preserve">'full Y data set, no transformations', </v>
       </c>
       <c r="N25" s="1">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O25" s="1">
         <f t="shared" si="7"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="P25" s="1">
         <f t="shared" si="7"/>
+        <v>35</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="S25" s="1">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="R25" s="1">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="S25" s="1">
-        <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
       <c r="T25" s="1">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="V25" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|10b                   |</v>
+        <v>|9                     |</v>
       </c>
       <c r="W25" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test_y01_vc01                     |</v>
+        <v>y01_df01                          |</v>
       </c>
       <c r="X25" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>test Y, no transformations                              |</v>
+        <v>full Y data set, no transformations                       |</v>
       </c>
       <c r="Y25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|10b                   |test_y01_vc01                     |test Y, no transformations                              |</v>
+        <v>|9                     |y01_df01                          |full Y data set, no transformations                       |</v>
       </c>
     </row>
     <row r="26" spans="4:25" x14ac:dyDescent="0.25">
       <c r="D26" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>197</v>
+        <v>142</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train Y, #6a/#10a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'train Y, no transformations', </v>
       </c>
       <c r="N26" s="1">
         <f t="shared" si="7"/>
@@ -6602,11 +6623,11 @@
       </c>
       <c r="O26" s="1">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="P26" s="1">
         <f t="shared" si="7"/>
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="R26" s="1">
         <f t="shared" si="4"/>
@@ -6614,97 +6635,93 @@
       </c>
       <c r="S26" s="1">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="T26" s="1">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="V26" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|10c                   |</v>
+        <v>|10a                   |</v>
       </c>
       <c r="W26" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_y01_vc01a                   |</v>
+        <v>train_y01_vc01                    |</v>
       </c>
       <c r="X26" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train Y, #6a/#10a + SMOTE rebalancing                   |</v>
+        <v>train Y, no transformations                               |</v>
       </c>
       <c r="Y26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|10c                   |train_y01_vc01a                   |train Y, #6a/#10a + SMOTE rebalancing                   |</v>
+        <v>|10a                   |train_y01_vc01                    |train Y, no transformations                               |</v>
       </c>
     </row>
     <row r="27" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D27" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>207</v>
-      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="F27" s="4"/>
       <c r="G27" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train Y, #7a/#10a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'', </v>
       </c>
       <c r="N27" s="1">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O27" s="1">
         <f t="shared" si="7"/>
+        <v>19</v>
+      </c>
+      <c r="P27" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="1">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="S27" s="1">
+        <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="P27" s="1">
-        <f t="shared" si="7"/>
-        <v>37</v>
-      </c>
-      <c r="R27" s="1">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-      <c r="S27" s="1">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
       <c r="T27" s="1">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="V27" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|10d                   |</v>
+        <v>|                      |</v>
       </c>
       <c r="W27" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_y01_vc01b                   |</v>
+        <v>train_y01_vc01_eda1               |</v>
       </c>
       <c r="X27" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train Y, #7a/#10a + SMOTE rebalancing                   |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|10d                   |train_y01_vc01b                   |train Y, #7a/#10a + SMOTE rebalancing                   |</v>
+        <v>|                      |train_y01_vc01_eda1               |                                                          |</v>
       </c>
     </row>
     <row r="28" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D28" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>208</v>
+      <c r="D28" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'train Y, #8a/#10a + SMOTE rebalancing', </v>
+        <v xml:space="preserve">'test Y, no transformations', </v>
       </c>
       <c r="N28" s="1">
         <f t="shared" si="7"/>
@@ -6712,11 +6729,11 @@
       </c>
       <c r="O28" s="1">
         <f t="shared" si="7"/>
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="P28" s="1">
         <f t="shared" si="7"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="R28" s="1">
         <f t="shared" si="4"/>
@@ -6724,174 +6741,192 @@
       </c>
       <c r="S28" s="1">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="T28" s="1">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="V28" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|10e                   |</v>
+        <v>|10b                   |</v>
       </c>
       <c r="W28" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train_y01_vc01c (IN PROCESS)      |</v>
+        <v>test_y01_vc01                     |</v>
       </c>
       <c r="X28" s="1" t="str">
         <f t="shared" si="6"/>
-        <v>train Y, #8a/#10a + SMOTE rebalancing                   |</v>
+        <v>test Y, no transformations                                |</v>
       </c>
       <c r="Y28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|10e                   |train_y01_vc01c (IN PROCESS)      |train Y, #8a/#10a + SMOTE rebalancing                   |</v>
+        <v>|10b                   |test_y01_vc01                     |test Y, no transformations                                |</v>
       </c>
     </row>
     <row r="29" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="D29" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>206</v>
+      </c>
       <c r="G29" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'', </v>
+        <v xml:space="preserve">'train Y, #6a/#10a + SMOTE rebalancing', </v>
       </c>
       <c r="N29" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O29" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P29" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="R29" s="1">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S29" s="1">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="T29" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="V29" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|                      |</v>
+        <v>|10c                   |</v>
       </c>
       <c r="W29" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                  |</v>
+        <v>train_y01_vc01a                   |</v>
       </c>
       <c r="X29" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v>train Y, #6a/#10a + SMOTE rebalancing                     |</v>
       </c>
       <c r="Y29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|10c                   |train_y01_vc01a                   |train Y, #6a/#10a + SMOTE rebalancing                     |</v>
       </c>
     </row>
     <row r="30" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
+      <c r="D30" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>207</v>
+      </c>
       <c r="G30" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'', </v>
+        <v xml:space="preserve">'train Y, #7a/#10a + SMOTE rebalancing', </v>
       </c>
       <c r="N30" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O30" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P30" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="R30" s="1">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S30" s="1">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="T30" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="V30" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|                      |</v>
+        <v>|10d                   |</v>
       </c>
       <c r="W30" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                  |</v>
+        <v>train_y01_vc01b                   |</v>
       </c>
       <c r="X30" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v>train Y, #7a/#10a + SMOTE rebalancing                     |</v>
       </c>
       <c r="Y30" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|10d                   |train_y01_vc01b                   |train Y, #7a/#10a + SMOTE rebalancing                     |</v>
       </c>
     </row>
     <row r="31" spans="4:25" x14ac:dyDescent="0.25">
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
+      <c r="D31" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="G31" s="1" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">'', </v>
+        <v xml:space="preserve">'train Y, #8a/#10a + SMOTE rebalancing', </v>
       </c>
       <c r="N31" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O31" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="P31" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="R31" s="1">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S31" s="1">
         <f t="shared" si="4"/>
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="T31" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="V31" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>|                      |</v>
+        <v>|10e                   |</v>
       </c>
       <c r="W31" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                  |</v>
+        <v>train_y01_vc01c (IN PROCESS)      |</v>
       </c>
       <c r="X31" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v>train Y, #8a/#10a + SMOTE rebalancing                     |</v>
       </c>
       <c r="Y31" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|10e                   |train_y01_vc01c (IN PROCESS)      |train Y, #8a/#10a + SMOTE rebalancing                     |</v>
       </c>
     </row>
     <row r="32" spans="4:25" x14ac:dyDescent="0.25">
@@ -6924,7 +6959,7 @@
       </c>
       <c r="T32" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V32" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6936,11 +6971,11 @@
       </c>
       <c r="X32" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y32" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="33" spans="4:25" x14ac:dyDescent="0.25">
@@ -6973,7 +7008,7 @@
       </c>
       <c r="T33" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V33" s="1" t="str">
         <f t="shared" si="5"/>
@@ -6985,11 +7020,11 @@
       </c>
       <c r="X33" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y33" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="34" spans="4:25" x14ac:dyDescent="0.25">
@@ -7022,7 +7057,7 @@
       </c>
       <c r="T34" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V34" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7034,11 +7069,11 @@
       </c>
       <c r="X34" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y34" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="35" spans="4:25" x14ac:dyDescent="0.25">
@@ -7071,7 +7106,7 @@
       </c>
       <c r="T35" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V35" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7083,11 +7118,11 @@
       </c>
       <c r="X35" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y35" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="36" spans="4:25" x14ac:dyDescent="0.25">
@@ -7120,7 +7155,7 @@
       </c>
       <c r="T36" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V36" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7132,11 +7167,11 @@
       </c>
       <c r="X36" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y36" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="37" spans="4:25" x14ac:dyDescent="0.25">
@@ -7169,7 +7204,7 @@
       </c>
       <c r="T37" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V37" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7181,11 +7216,11 @@
       </c>
       <c r="X37" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y37" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="38" spans="4:25" x14ac:dyDescent="0.25">
@@ -7218,7 +7253,7 @@
       </c>
       <c r="T38" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V38" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7230,11 +7265,11 @@
       </c>
       <c r="X38" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y38" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="39" spans="4:25" x14ac:dyDescent="0.25">
@@ -7267,7 +7302,7 @@
       </c>
       <c r="T39" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V39" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7279,11 +7314,11 @@
       </c>
       <c r="X39" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y39" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="40" spans="4:25" x14ac:dyDescent="0.25">
@@ -7316,7 +7351,7 @@
       </c>
       <c r="T40" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V40" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7328,11 +7363,11 @@
       </c>
       <c r="X40" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y40" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="41" spans="4:25" x14ac:dyDescent="0.25">
@@ -7365,7 +7400,7 @@
       </c>
       <c r="T41" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V41" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7377,11 +7412,11 @@
       </c>
       <c r="X41" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y41" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="42" spans="4:25" x14ac:dyDescent="0.25">
@@ -7414,7 +7449,7 @@
       </c>
       <c r="T42" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V42" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7426,11 +7461,11 @@
       </c>
       <c r="X42" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y42" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="43" spans="4:25" x14ac:dyDescent="0.25">
@@ -7463,7 +7498,7 @@
       </c>
       <c r="T43" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V43" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7475,11 +7510,11 @@
       </c>
       <c r="X43" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y43" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="44" spans="4:25" x14ac:dyDescent="0.25">
@@ -7512,7 +7547,7 @@
       </c>
       <c r="T44" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V44" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7524,11 +7559,11 @@
       </c>
       <c r="X44" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y44" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="45" spans="4:25" x14ac:dyDescent="0.25">
@@ -7561,7 +7596,7 @@
       </c>
       <c r="T45" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V45" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7573,11 +7608,11 @@
       </c>
       <c r="X45" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y45" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="46" spans="4:25" x14ac:dyDescent="0.25">
@@ -7610,7 +7645,7 @@
       </c>
       <c r="T46" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V46" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7622,11 +7657,11 @@
       </c>
       <c r="X46" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y46" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="47" spans="4:25" x14ac:dyDescent="0.25">
@@ -7659,7 +7694,7 @@
       </c>
       <c r="T47" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V47" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7671,11 +7706,11 @@
       </c>
       <c r="X47" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y47" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="48" spans="4:25" x14ac:dyDescent="0.25">
@@ -7708,7 +7743,7 @@
       </c>
       <c r="T48" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V48" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7720,11 +7755,11 @@
       </c>
       <c r="X48" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y48" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="49" spans="4:25" x14ac:dyDescent="0.25">
@@ -7757,7 +7792,7 @@
       </c>
       <c r="T49" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V49" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7769,11 +7804,11 @@
       </c>
       <c r="X49" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y49" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="50" spans="4:25" x14ac:dyDescent="0.25">
@@ -7806,7 +7841,7 @@
       </c>
       <c r="T50" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V50" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7818,11 +7853,11 @@
       </c>
       <c r="X50" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y50" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="51" spans="4:25" x14ac:dyDescent="0.25">
@@ -7855,7 +7890,7 @@
       </c>
       <c r="T51" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V51" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7867,11 +7902,11 @@
       </c>
       <c r="X51" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y51" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="52" spans="4:25" x14ac:dyDescent="0.25">
@@ -7904,7 +7939,7 @@
       </c>
       <c r="T52" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V52" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7916,11 +7951,11 @@
       </c>
       <c r="X52" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y52" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="53" spans="4:25" x14ac:dyDescent="0.25">
@@ -7953,7 +7988,7 @@
       </c>
       <c r="T53" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V53" s="1" t="str">
         <f t="shared" si="5"/>
@@ -7965,11 +8000,11 @@
       </c>
       <c r="X53" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y53" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="54" spans="4:25" x14ac:dyDescent="0.25">
@@ -8002,7 +8037,7 @@
       </c>
       <c r="T54" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V54" s="1" t="str">
         <f t="shared" si="5"/>
@@ -8014,11 +8049,11 @@
       </c>
       <c r="X54" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y54" s="1" t="str">
-        <f t="shared" ref="Y54:Y116" si="8">V54&amp;W54&amp;X54</f>
-        <v>|                      |                                  |                                                        |</v>
+        <f t="shared" ref="Y54" si="8">V54&amp;W54&amp;X54</f>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
     <row r="55" spans="4:25" x14ac:dyDescent="0.25">
@@ -8051,7 +8086,7 @@
       </c>
       <c r="T55" s="1">
         <f t="shared" si="4"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V55" s="1" t="str">
         <f t="shared" si="5"/>
@@ -8063,11 +8098,11 @@
       </c>
       <c r="X55" s="1" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">                                                        |</v>
+        <v xml:space="preserve">                                                          |</v>
       </c>
       <c r="Y55" s="1" t="str">
         <f>V55&amp;W55&amp;X55</f>
-        <v>|                      |                                  |                                                        |</v>
+        <v>|                      |                                  |                                                          |</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on finalization of codebook
updated file names, updated some ref docs, cleaning up jupyter notebook in order to finalize it
</commit_message>
<xml_diff>
--- a/ref_docs/Feature_Map_v1.xlsx
+++ b/ref_docs/Feature_Map_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarr\Documents\GitHub\ads505_business_proj\ref_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3801EC8-79C1-4AB9-B3E6-DE3CC8D2C145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A34EAB3-56C4-43B3-BE27-BAED0FA17CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="1080" windowWidth="25005" windowHeight="13905" activeTab="1" xr2:uid="{9E5FB942-D815-48B7-87F6-15AD5525091B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{9E5FB942-D815-48B7-87F6-15AD5525091B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5304,7 +5304,7 @@
   <dimension ref="D1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>